<commit_message>
update fr excel template, fix bug when deleting zone
</commit_message>
<xml_diff>
--- a/static/template_fr.xlsx
+++ b/static/template_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8925A8A-05EC-D044-857D-EB9FDF9F408B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4B67EA-811B-D247-BD21-2C3C7FC6A013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="32640" windowHeight="20880" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quote" sheetId="58" r:id="rId1"/>
@@ -12215,6 +12215,27 @@
     <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12226,15 +12247,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -12263,7 +12275,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="3" fillId="24" borderId="11" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12299,35 +12323,11 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -12762,8 +12762,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:J48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13394,13 +13394,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="89"/>
-      <c r="G5" s="121">
+      <c r="G5" s="129">
         <f ca="1">NOW()</f>
-        <v>45321.732523842591</v>
+        <v>45334.444553703703</v>
       </c>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="122"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="130"/>
     </row>
     <row r="6" spans="1:13" ht="55" customHeight="1">
       <c r="B6" s="94" t="s">
@@ -13425,10 +13425,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="93"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="124"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="132"/>
     </row>
     <row r="8" spans="1:13" ht="14">
       <c r="C8" s="62">
@@ -13436,22 +13436,22 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="6" customFormat="1" ht="14">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="126"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="126"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="134"/>
     </row>
     <row r="10" spans="1:13" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A10" s="55" t="s">
@@ -13461,15 +13461,15 @@
       <c r="C10" s="81">
         <v>10</v>
       </c>
-      <c r="D10" s="128" t="s">
+      <c r="D10" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
-      <c r="H10" s="129"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="130"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="138"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="31" t="s">
@@ -13479,10 +13479,10 @@
       <c r="C11" s="81">
         <v>250</v>
       </c>
-      <c r="D11" s="131"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
       <c r="H11" s="33"/>
       <c r="J11" s="7"/>
     </row>
@@ -13494,9 +13494,9 @@
       <c r="C12" s="81">
         <v>0</v>
       </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
@@ -13510,24 +13510,24 @@
       <c r="C13" s="81">
         <v>12</v>
       </c>
-      <c r="D13" s="108"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110"/>
+      <c r="D13" s="124"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="126"/>
       <c r="M13" s="62" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="115" t="s">
+      <c r="A15" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="117"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="121"/>
       <c r="E15" s="44" t="s">
         <v>10</v>
       </c>
@@ -13550,26 +13550,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="113"/>
-      <c r="H16" s="113"/>
-      <c r="I16" s="113"/>
-      <c r="J16" s="114"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="118"/>
     </row>
     <row r="17" spans="1:11" ht="122" customHeight="1">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="28">
         <v>10</v>
       </c>
@@ -13824,8 +13824,8 @@
       <c r="J33" s="25"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="106"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="114"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
@@ -13836,8 +13836,8 @@
       <c r="J34" s="27"/>
     </row>
     <row r="35" spans="1:10" ht="14">
-      <c r="A35" s="134"/>
-      <c r="B35" s="135" t="s">
+      <c r="A35" s="104"/>
+      <c r="B35" s="105" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="70" t="s">
@@ -13852,8 +13852,8 @@
       <c r="J35" s="71"/>
     </row>
     <row r="36" spans="1:10" ht="14">
-      <c r="A36" s="136"/>
-      <c r="B36" s="137" t="s">
+      <c r="A36" s="106"/>
+      <c r="B36" s="107" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="70" t="s">
@@ -13868,8 +13868,8 @@
       <c r="J36" s="71"/>
     </row>
     <row r="37" spans="1:10" ht="14">
-      <c r="A37" s="138"/>
-      <c r="B37" s="139" t="s">
+      <c r="A37" s="108"/>
+      <c r="B37" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C37" s="70" t="s">
@@ -13972,7 +13972,7 @@
       <c r="C49" s="37"/>
     </row>
     <row r="50" spans="1:10" ht="15">
-      <c r="A50" s="140" t="s">
+      <c r="A50" s="110" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="36"/>
@@ -13996,10 +13996,10 @@
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
-      <c r="G51" s="104"/>
-      <c r="H51" s="104"/>
-      <c r="I51" s="104"/>
-      <c r="J51" s="105"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="112"/>
     </row>
     <row r="52" spans="1:10" ht="14">
       <c r="A52" s="68"/>
@@ -14007,10 +14007,10 @@
       <c r="C52" s="37"/>
       <c r="D52" s="5"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="104"/>
-      <c r="H52" s="104"/>
-      <c r="I52" s="104"/>
-      <c r="J52" s="105"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="112"/>
     </row>
     <row r="53" spans="1:10" ht="14">
       <c r="A53" s="67"/>
@@ -14235,9 +14235,8 @@
       <c r="A87" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A48:J48"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14265,6 +14264,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14314,7 +14322,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
@@ -14326,7 +14334,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14499,16 +14507,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -14516,7 +14523,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14526,7 +14533,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14542,12 +14549,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix template excel floating precision in total
</commit_message>
<xml_diff>
--- a/static/template_fr.xlsx
+++ b/static/template_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAC8152-9C13-D74C-8681-A697B1AE83B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D00FB5-9BB8-434E-A0EE-5FA8B90E5F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12267,6 +12267,48 @@
     <xf numFmtId="2" fontId="44" fillId="24" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12307,48 +12349,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12785,7 +12785,7 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13470,13 +13470,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="85"/>
-      <c r="G5" s="116">
+      <c r="G5" s="130">
         <f ca="1">NOW()</f>
-        <v>45938.660065856478</v>
+        <v>45938.733312615739</v>
       </c>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="117"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
     </row>
     <row r="6" spans="1:21" ht="55" customHeight="1">
       <c r="B6" s="90" t="s">
@@ -13495,50 +13495,50 @@
         <v>2</v>
       </c>
       <c r="F7" s="89"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="119"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="133"/>
     </row>
     <row r="9" spans="1:21" s="6" customFormat="1" ht="14">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="121"/>
-      <c r="D9" s="120" t="s">
+      <c r="B9" s="135"/>
+      <c r="D9" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="121"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="135"/>
     </row>
     <row r="10" spans="1:21" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A10" s="55" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="56"/>
-      <c r="D10" s="123" t="s">
+      <c r="D10" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="125"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="139"/>
     </row>
     <row r="11" spans="1:21" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="32"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
       <c r="H11" s="33"/>
       <c r="J11" s="7"/>
     </row>
@@ -13547,9 +13547,9 @@
         <v>7</v>
       </c>
       <c r="B12" s="35"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
@@ -13560,13 +13560,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="127"/>
       <c r="M13" s="61" t="s">
         <v>41</v>
       </c>
@@ -13575,12 +13575,12 @@
       <c r="L14" s="109"/>
     </row>
     <row r="15" spans="1:21" s="6" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="136"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="122"/>
       <c r="E15" s="44" t="s">
         <v>10</v>
       </c>
@@ -13603,26 +13603,26 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="18" customHeight="1">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="133"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="119"/>
     </row>
     <row r="17" spans="1:11" ht="122" customHeight="1">
-      <c r="A17" s="137" t="s">
+      <c r="A17" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
       <c r="E17" s="28">
         <v>10</v>
       </c>
@@ -13877,8 +13877,8 @@
       <c r="J33" s="25"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="128"/>
-      <c r="B34" s="129"/>
+      <c r="A34" s="114"/>
+      <c r="B34" s="115"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
@@ -14258,11 +14258,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="D13:J13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14270,6 +14265,11 @@
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:G11"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="D13:J13"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -14280,6 +14280,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14329,16 +14338,19 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14511,19 +14523,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -14531,15 +14539,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14555,14 +14565,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>